<commit_message>
Parameter-Variation for MtoBscan.m added
</commit_message>
<xml_diff>
--- a/Ausarbeitung/Charts.xlsx
+++ b/Ausarbeitung/Charts.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="MtoBScan Var" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>Rohdatenverarbeitung.m</t>
   </si>
@@ -42,6 +43,102 @@
   </si>
   <si>
     <t>Anzahl Parameter</t>
+  </si>
+  <si>
+    <t>Variation der Parameter bei MtoBScan</t>
+  </si>
+  <si>
+    <t>Diese wurden einzeln (nicht in Kombination!) variiert und es wurde geprüft ob das Ergebnis beim ASCAN3 von 0-10000 noch stimmt</t>
+  </si>
+  <si>
+    <t>Parameter</t>
+  </si>
+  <si>
+    <t>Agenda: 1 - ja, 0.5 - ungenau, 0 - keine Ergebnisse</t>
+  </si>
+  <si>
+    <t>+1</t>
+  </si>
+  <si>
+    <t>+2</t>
+  </si>
+  <si>
+    <t>+3</t>
+  </si>
+  <si>
+    <t>+4</t>
+  </si>
+  <si>
+    <t>+5</t>
+  </si>
+  <si>
+    <t>+6</t>
+  </si>
+  <si>
+    <t>+7</t>
+  </si>
+  <si>
+    <t>+8</t>
+  </si>
+  <si>
+    <t>+9</t>
+  </si>
+  <si>
+    <t>+10</t>
+  </si>
+  <si>
+    <t>-1</t>
+  </si>
+  <si>
+    <t>-2</t>
+  </si>
+  <si>
+    <t>-3</t>
+  </si>
+  <si>
+    <t>-4</t>
+  </si>
+  <si>
+    <t>-5</t>
+  </si>
+  <si>
+    <t>-6</t>
+  </si>
+  <si>
+    <t>-7</t>
+  </si>
+  <si>
+    <t>-8</t>
+  </si>
+  <si>
+    <t>-9</t>
+  </si>
+  <si>
+    <t>Lbound Scanline</t>
+  </si>
+  <si>
+    <t>Ubound Scanline</t>
+  </si>
+  <si>
+    <t>Lbound Line</t>
+  </si>
+  <si>
+    <t>Ubound Line</t>
+  </si>
+  <si>
+    <t>Param Line</t>
+  </si>
+  <si>
+    <t>LBound Prewitt</t>
+  </si>
+  <si>
+    <t>Ubound Prewitt</t>
+  </si>
+  <si>
+    <t>Current Value</t>
+  </si>
+  <si>
+    <t>Distance Param</t>
   </si>
 </sst>
 </file>
@@ -77,8 +174,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -136,7 +234,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -957,16 +1054,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>12699</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>50799</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>241299</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>101599</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>295274</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>53974</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>523874</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>104774</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1253,7 +1350,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -1307,4 +1404,663 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="14.36328125" customWidth="1"/>
+    <col min="2" max="2" width="11.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.26953125" customWidth="1"/>
+    <col min="4" max="4" width="13.453125" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="6" max="6" width="14.81640625" customWidth="1"/>
+    <col min="7" max="8" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.90625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" t="s">
+        <v>35</v>
+      </c>
+      <c r="G6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H6" t="s">
+        <v>30</v>
+      </c>
+      <c r="I6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>3</v>
+      </c>
+      <c r="E7">
+        <v>4</v>
+      </c>
+      <c r="F7">
+        <v>7</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>3</v>
+      </c>
+      <c r="E8">
+        <v>5</v>
+      </c>
+      <c r="F8">
+        <v>7</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>3</v>
+      </c>
+      <c r="E9">
+        <v>4</v>
+      </c>
+      <c r="F9">
+        <v>7</v>
+      </c>
+      <c r="H9">
+        <v>5</v>
+      </c>
+      <c r="I9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>3</v>
+      </c>
+      <c r="E10">
+        <v>3</v>
+      </c>
+      <c r="F10">
+        <v>7</v>
+      </c>
+      <c r="H10">
+        <v>2</v>
+      </c>
+      <c r="I10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>4</v>
+      </c>
+      <c r="F11">
+        <v>7</v>
+      </c>
+      <c r="H11">
+        <v>3</v>
+      </c>
+      <c r="I11">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12">
+        <v>7</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <v>4</v>
+      </c>
+      <c r="F12">
+        <v>7</v>
+      </c>
+      <c r="H12">
+        <v>2</v>
+      </c>
+      <c r="I12">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>7</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>4</v>
+      </c>
+      <c r="F13">
+        <v>7</v>
+      </c>
+      <c r="H13">
+        <v>3</v>
+      </c>
+      <c r="I13">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14">
+        <v>7</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>7</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>7</v>
+      </c>
+      <c r="E15">
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <v>7</v>
+      </c>
+      <c r="G15">
+        <v>7</v>
+      </c>
+      <c r="H15">
+        <v>5</v>
+      </c>
+      <c r="I15">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>7</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>7</v>
+      </c>
+      <c r="E16">
+        <v>2</v>
+      </c>
+      <c r="F16">
+        <v>7</v>
+      </c>
+      <c r="G16">
+        <v>7</v>
+      </c>
+      <c r="H16">
+        <v>1</v>
+      </c>
+      <c r="I16">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>7</v>
+      </c>
+      <c r="E17">
+        <v>7</v>
+      </c>
+      <c r="F17">
+        <v>7</v>
+      </c>
+      <c r="G17">
+        <v>7</v>
+      </c>
+      <c r="H17">
+        <v>7</v>
+      </c>
+      <c r="I17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18">
+        <v>7</v>
+      </c>
+      <c r="C18">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>7</v>
+      </c>
+      <c r="E18">
+        <v>2</v>
+      </c>
+      <c r="F18">
+        <v>7</v>
+      </c>
+      <c r="G18">
+        <v>7</v>
+      </c>
+      <c r="H18">
+        <v>2</v>
+      </c>
+      <c r="I18">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>7</v>
+      </c>
+      <c r="C19">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>6</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>7</v>
+      </c>
+      <c r="G19">
+        <v>7</v>
+      </c>
+      <c r="I19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>7</v>
+      </c>
+      <c r="C20">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>5</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>7</v>
+      </c>
+      <c r="G20">
+        <v>7</v>
+      </c>
+      <c r="I20">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>7</v>
+      </c>
+      <c r="C21">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>4</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>7</v>
+      </c>
+      <c r="I21">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>7</v>
+      </c>
+      <c r="D22">
+        <v>3</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>7</v>
+      </c>
+      <c r="I22">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>7</v>
+      </c>
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="I23">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>7</v>
+      </c>
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24">
+        <v>7</v>
+      </c>
+      <c r="I24">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25">
+        <v>6</v>
+      </c>
+      <c r="I25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>7</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>6</v>
+      </c>
+      <c r="I26">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="1">
+        <v>-10</v>
+      </c>
+      <c r="B27">
+        <v>7</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>4</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="I27">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E7:E27">
+    <cfRule type="colorScale" priority="7">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7:F27">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:F27">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7:H27">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFFEF9C"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:C27 E7:H27">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:H27">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:I27">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>